<commit_message>
Add food limit xlsx.
</commit_message>
<xml_diff>
--- a/data/Food.xlsx
+++ b/data/Food.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37320" windowHeight="22680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1253,11 +1253,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1276,7 +1276,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1284,7 +1284,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1294,6 +1294,12 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1313,8 +1319,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1391,76 +1399,78 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="69">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="71">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -15813,6 +15823,7 @@
       <c r="B101" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -15830,7 +15841,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16172,7 +16183,7 @@
         <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C3" t="s">
         <v>246</v>
@@ -29853,6 +29864,7 @@
       <sortCondition descending="1" ref="G1:G89"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>